<commit_message>
feat: complete Sprint 2 backlog and finalize fall semester date updates
</commit_message>
<xml_diff>
--- a/Sprint 1 Backlog.xlsx
+++ b/Sprint 1 Backlog.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montay\OneDrive\Documents\ITSC 3155\Restaurant-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666B2C6C-34C0-4AE9-BBBE-209519B544E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E913C0-FB16-4246-B323-06C516BF50B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="63">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
   <si>
-    <t>Sprint Backlog</t>
-  </si>
-  <si>
     <t>Story Tasks</t>
   </si>
   <si>
@@ -159,6 +157,72 @@
   </si>
   <si>
     <t>S1-T19 Seed Sample Data</t>
+  </si>
+  <si>
+    <t>S2-T1 Add promotion_id support to menu-items</t>
+  </si>
+  <si>
+    <t>S2-T2 Add average rating to menu-item GET response</t>
+  </si>
+  <si>
+    <t>S2-T3 Add payments CRUD endpoints</t>
+  </si>
+  <si>
+    <t>S2-T4 Integrate payments into order creation</t>
+  </si>
+  <si>
+    <t>S2-T5 Apply promotion discount to order total</t>
+  </si>
+  <si>
+    <t>S2-T6 Add final price calculation</t>
+  </si>
+  <si>
+    <t>S2-T7 Add order status update endpoint</t>
+  </si>
+  <si>
+    <t>S2-T8 Add date filter to GET /orders</t>
+  </si>
+  <si>
+    <t>S2-T9 Add sorting (price/date) to orders</t>
+  </si>
+  <si>
+    <t>S2-T10 Add order summary fields (item count, discount, totals)</t>
+  </si>
+  <si>
+    <t>S2-T11 Add promotions CRUD</t>
+  </si>
+  <si>
+    <t>S2-T12 Add reviews CRUD</t>
+  </si>
+  <si>
+    <t>S2-T13 Add validation for all request bodies</t>
+  </si>
+  <si>
+    <t>S2-T14 Add missing DELETE endpoints</t>
+  </si>
+  <si>
+    <t>S2-T15 Add DB indexes for performance</t>
+  </si>
+  <si>
+    <t>S2-T16 Add join relationships (orders ↔ order_details)</t>
+  </si>
+  <si>
+    <t>S2-T17 Final DB validation + seed refresh</t>
+  </si>
+  <si>
+    <t>Order Placement</t>
+  </si>
+  <si>
+    <t>Order Management Dashboard</t>
+  </si>
+  <si>
+    <t>API Development / CRUD</t>
+  </si>
+  <si>
+    <t>Sprint Backlog NOV 17 - 21</t>
+  </si>
+  <si>
+    <t>Sprint Backlog Nov 24 - 28</t>
   </si>
 </sst>
 </file>
@@ -328,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +446,48 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -633,7 +739,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -649,92 +755,92 @@
     </row>
     <row r="3" spans="1:12" ht="12.75">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.25">
       <c r="A4" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>8</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:J4" si="0">SUM(D5:D8)</f>
+        <f>SUM(D5:D8)</f>
         <v>9</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E5:E8)</f>
         <v>2</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(F5:F8)</f>
         <v>3</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(G5:G8)</f>
         <v>2</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(H5:H8)</f>
         <v>2</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(I5:I8)</f>
         <v>2</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(J5:J8)</f>
         <v>2</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="25.5">
       <c r="A5" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6">
         <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8">
         <v>3</v>
@@ -758,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" s="8">
         <v>1</v>
@@ -766,13 +872,13 @@
     </row>
     <row r="6" spans="1:12" ht="25.5">
       <c r="A6" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6">
         <v>8</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
@@ -796,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>1</v>
@@ -804,13 +910,13 @@
     </row>
     <row r="7" spans="1:12" ht="25.5">
       <c r="A7" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6">
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="8">
         <v>2</v>
@@ -834,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" s="8">
         <v>1</v>
@@ -842,13 +948,13 @@
     </row>
     <row r="8" spans="1:12" ht="25.5">
       <c r="A8" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6">
         <v>8</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="8">
         <v>2</v>
@@ -872,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="8">
         <v>1</v>
@@ -880,7 +986,7 @@
     </row>
     <row r="9" spans="1:12" ht="26.25">
       <c r="A9" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>13</v>
@@ -915,19 +1021,19 @@
         <v>0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="25.5">
       <c r="A10" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6">
         <v>13</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="8">
         <v>3</v>
@@ -951,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="8">
         <v>1</v>
@@ -959,13 +1065,13 @@
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6">
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="8">
         <v>2</v>
@@ -989,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" s="8">
         <v>1</v>
@@ -997,13 +1103,13 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6">
         <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="8">
         <v>3</v>
@@ -1027,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" s="8">
         <v>1</v>
@@ -1035,54 +1141,54 @@
     </row>
     <row r="13" spans="1:12" ht="26.25">
       <c r="A13" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:J13" si="1">SUM(D14:D17)</f>
+        <f t="shared" ref="D13:J13" si="0">SUM(D14:D17)</f>
         <v>12</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="25.5">
       <c r="A14" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6">
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="8">
         <v>4</v>
@@ -1106,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L14" s="8">
         <v>1</v>
@@ -1114,13 +1220,13 @@
     </row>
     <row r="15" spans="1:12" ht="12.75">
       <c r="A15" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6">
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="8">
         <v>3</v>
@@ -1144,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L15" s="8">
         <v>1</v>
@@ -1152,13 +1258,13 @@
     </row>
     <row r="16" spans="1:12" ht="25.5">
       <c r="A16" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6">
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="8">
         <v>3</v>
@@ -1182,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" s="8">
         <v>1</v>
@@ -1190,13 +1296,13 @@
     </row>
     <row r="17" spans="1:12" ht="25.5">
       <c r="A17" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6">
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="8">
         <v>2</v>
@@ -1220,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L17" s="8">
         <v>1</v>
@@ -1228,7 +1334,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -1263,19 +1369,19 @@
         <v>0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6">
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="8">
         <v>2</v>
@@ -1299,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="8">
         <v>1</v>
@@ -1307,13 +1413,13 @@
     </row>
     <row r="20" spans="1:12" ht="25.5">
       <c r="A20" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="6">
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
@@ -1337,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L20" s="8">
         <v>1</v>
@@ -1345,13 +1451,13 @@
     </row>
     <row r="21" spans="1:12" ht="25.5">
       <c r="A21" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="6">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="8">
         <v>2</v>
@@ -1375,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L21" s="8">
         <v>1</v>
@@ -1383,13 +1489,13 @@
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="6">
         <v>8</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="8">
         <v>2</v>
@@ -1413,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L22" s="8">
         <v>1</v>
@@ -1421,13 +1527,13 @@
     </row>
     <row r="23" spans="1:12" ht="38.25">
       <c r="A23" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="23">
         <v>8</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="22">
         <v>3</v>
@@ -1451,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L23" s="22">
         <v>1</v>
@@ -1459,7 +1565,7 @@
     </row>
     <row r="24" spans="1:12" ht="26.25">
       <c r="A24" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3">
         <v>5</v>
@@ -1494,19 +1600,19 @@
         <v>0</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="6">
         <v>5</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" s="8">
         <v>2</v>
@@ -1530,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L25" s="8">
         <v>1</v>
@@ -1538,13 +1644,13 @@
     </row>
     <row r="26" spans="1:12" ht="25.5">
       <c r="A26" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="6">
         <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="8">
         <v>2</v>
@@ -1568,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" s="8">
         <v>1</v>
@@ -1576,13 +1682,13 @@
     </row>
     <row r="27" spans="1:12" ht="25.5">
       <c r="A27" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="6">
         <v>5</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="8">
         <v>1</v>
@@ -1606,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L27" s="8">
         <v>1</v>
@@ -1614,7 +1720,7 @@
     </row>
     <row r="28" spans="1:12" ht="12.75">
       <c r="A28" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1658,11 +1764,1025 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K27" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K9:K27 K4:K8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"To Do,Doing,Done"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2277E5-F34C-48B9-8BB9-96917F3B1E32}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="20" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" style="20"/>
+    <col min="4" max="4" width="14.7109375" style="20" customWidth="1"/>
+    <col min="5" max="11" width="12.5703125" style="20"/>
+    <col min="12" max="12" width="13.85546875" style="20" customWidth="1"/>
+    <col min="13" max="16384" width="12.5703125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="14.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.25">
+      <c r="A2" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" ht="25.5">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="26.25">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="31">
+        <v>5</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="32">
+        <v>4</v>
+      </c>
+      <c r="E4" s="32">
+        <f>SUM(E5:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="32">
+        <f>SUM(F5:F6)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="32">
+        <f>SUM(G5:G6)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="32">
+        <f>SUM(H5:H6)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="32">
+        <f>SUM(I5:I6)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="32">
+        <f>SUM(J5:J6)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" ht="51">
+      <c r="A5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="34">
+        <v>5</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="38.25">
+      <c r="A6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="34">
+        <v>5</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1</v>
+      </c>
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
+      <c r="A7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="31">
+        <v>13</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="32">
+        <f t="shared" ref="D7:J7" si="0">SUM(D8:D11)</f>
+        <v>10</v>
+      </c>
+      <c r="E7" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H7" s="32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="32">
+        <f>SUM(L5:L6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="38.25">
+      <c r="A8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="34">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="19">
+        <v>4</v>
+      </c>
+      <c r="E8" s="19">
+        <v>2</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="38.25">
+      <c r="A9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="34">
+        <v>13</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1</v>
+      </c>
+      <c r="H9" s="19">
+        <v>1</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
+        <v>0</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="38.25">
+      <c r="A10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="34">
+        <v>13</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19">
+        <v>2</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <v>1</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="25.5">
+      <c r="A11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="34">
+        <v>13</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19">
+        <v>0</v>
+      </c>
+      <c r="H11" s="19">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19">
+        <v>1</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="39">
+      <c r="A12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="31">
+        <v>5</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="32">
+        <f t="shared" ref="D12:J12" si="1">SUM(D13:D16)</f>
+        <v>10</v>
+      </c>
+      <c r="E12" s="32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="32">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H12" s="32">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I12" s="32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="32">
+        <f>SUM(L8:L11)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="38.25">
+      <c r="A13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="34">
+        <v>5</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="19">
+        <v>3</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1</v>
+      </c>
+      <c r="G13" s="19">
+        <v>1</v>
+      </c>
+      <c r="H13" s="19">
+        <v>0</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0</v>
+      </c>
+      <c r="K13" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="25.5">
+      <c r="A14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="34">
+        <v>5</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="19">
+        <v>2</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1</v>
+      </c>
+      <c r="F14" s="19">
+        <v>3</v>
+      </c>
+      <c r="G14" s="19">
+        <v>3</v>
+      </c>
+      <c r="H14" s="19">
+        <v>3</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="38.25">
+      <c r="A15" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="34">
+        <v>5</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="19">
+        <v>2</v>
+      </c>
+      <c r="E15" s="19">
+        <v>0</v>
+      </c>
+      <c r="F15" s="19">
+        <v>0</v>
+      </c>
+      <c r="G15" s="19">
+        <v>1</v>
+      </c>
+      <c r="H15" s="19">
+        <v>1</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+      <c r="J15" s="19">
+        <v>0</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="51">
+      <c r="A16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="34">
+        <v>5</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="19">
+        <v>3</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="19">
+        <v>2</v>
+      </c>
+      <c r="J16" s="19">
+        <v>0</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="26.25">
+      <c r="A17" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="31">
+        <v>13</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="32">
+        <f t="shared" ref="D17:J17" si="2">SUM(D18:D21)</f>
+        <v>14</v>
+      </c>
+      <c r="E17" s="32">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="32">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H17" s="32">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I17" s="32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="32">
+        <f>SUM(L13:L16)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="25.5">
+      <c r="A18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="34">
+        <v>13</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="19">
+        <v>4</v>
+      </c>
+      <c r="E18" s="19">
+        <v>2</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5">
+      <c r="A19" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="34">
+        <v>13</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="19">
+        <v>4</v>
+      </c>
+      <c r="E19" s="19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="38.25">
+      <c r="A20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="34">
+        <v>13</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="19">
+        <v>3</v>
+      </c>
+      <c r="E20" s="19">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1</v>
+      </c>
+      <c r="G20" s="19">
+        <v>1</v>
+      </c>
+      <c r="H20" s="19">
+        <v>1</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="38.25">
+      <c r="A21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="34">
+        <v>13</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="19">
+        <v>3</v>
+      </c>
+      <c r="E21" s="19">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0</v>
+      </c>
+      <c r="G21" s="19">
+        <v>1</v>
+      </c>
+      <c r="H21" s="19">
+        <v>1</v>
+      </c>
+      <c r="I21" s="19">
+        <v>1</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="26.25">
+      <c r="A22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="31">
+        <v>8</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="32">
+        <f>SUM(D23:D25)</f>
+        <v>8</v>
+      </c>
+      <c r="E22" s="32">
+        <f>SUM(E23:E25)</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="32">
+        <f>SUM(F23:F25)</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="32">
+        <f>SUM(G23:G25)</f>
+        <v>2</v>
+      </c>
+      <c r="H22" s="32">
+        <f>SUM(H23:H25)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="32">
+        <f>SUM(I23:I25)</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="32">
+        <f>SUM(J23:J25)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="32">
+        <f>SUM(L18:L21)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="38.25">
+      <c r="A23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="34">
+        <v>8</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="19">
+        <v>2</v>
+      </c>
+      <c r="E23" s="19">
+        <v>1</v>
+      </c>
+      <c r="F23" s="19">
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <v>0</v>
+      </c>
+      <c r="H23" s="19">
+        <v>0</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0</v>
+      </c>
+      <c r="J23" s="19">
+        <v>0</v>
+      </c>
+      <c r="K23" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="51">
+      <c r="A24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="34">
+        <v>8</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="19">
+        <v>3</v>
+      </c>
+      <c r="E24" s="19">
+        <v>1</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0</v>
+      </c>
+      <c r="G24" s="19">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19">
+        <v>1</v>
+      </c>
+      <c r="I24" s="19">
+        <v>0</v>
+      </c>
+      <c r="J24" s="19">
+        <v>0</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="38.25">
+      <c r="A25" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="34">
+        <v>8</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="19">
+        <v>3</v>
+      </c>
+      <c r="E25" s="19">
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
+        <v>1</v>
+      </c>
+      <c r="H25" s="19">
+        <v>0</v>
+      </c>
+      <c r="I25" s="19">
+        <v>1</v>
+      </c>
+      <c r="J25" s="19">
+        <v>0</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37">
+        <f>D4+D7+D12+D17+D22</f>
+        <v>46</v>
+      </c>
+      <c r="E26" s="37">
+        <f>E4+E7+E12+E17+E22</f>
+        <v>10</v>
+      </c>
+      <c r="F26" s="37">
+        <f>F4+F7+F12+F17+F22</f>
+        <v>12</v>
+      </c>
+      <c r="G26" s="37">
+        <f>G4+G7+G12+G17+G22</f>
+        <v>15</v>
+      </c>
+      <c r="H26" s="37">
+        <f>H4+H7+H12+H17+H22</f>
+        <v>13</v>
+      </c>
+      <c r="I26" s="37">
+        <f>I4+I7+I12+I17+I22</f>
+        <v>7</v>
+      </c>
+      <c r="J26" s="37">
+        <f>J4+J7+J12+J17+J22</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="36"/>
+      <c r="L26" s="37">
+        <f>SUM(L22,L17,L12,L7)</f>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K25" xr:uid="{FD3B23BF-4853-4659-9912-20F6DD4056B4}">
+      <formula1>"To Do,Doing,Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: completed sprint backlogs
</commit_message>
<xml_diff>
--- a/Sprint 1 Backlog.xlsx
+++ b/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montay\OneDrive\Documents\ITSC 3155\Restaurant-API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Final Project\Restaurant-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E913C0-FB16-4246-B323-06C516BF50B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D3F4E4-4BB3-491A-806D-96227B813DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -416,6 +416,55 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,37 +474,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -464,30 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,36 +722,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="15"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="12.75">
       <c r="A3" s="1" t="s">
@@ -792,7 +792,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="3">
@@ -800,31 +800,31 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4">
-        <f>SUM(D5:D8)</f>
+        <f t="shared" ref="D4:J4" si="0">SUM(D5:D8)</f>
         <v>9</v>
       </c>
       <c r="E4" s="4">
-        <f>SUM(E5:E8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F4" s="4">
-        <f>SUM(F5:F8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G4" s="4">
-        <f>SUM(G5:G8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H4" s="4">
-        <f>SUM(H5:H8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I4" s="4">
-        <f>SUM(I5:I8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J4" s="4">
-        <f>SUM(J5:J8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -833,7 +833,7 @@
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="25.5">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="6">
@@ -871,7 +871,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="25.5">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="6">
@@ -909,7 +909,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="25.5">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6">
@@ -947,7 +947,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="25.5">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="6">
@@ -974,7 +974,7 @@
       <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="14">
         <v>1</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -985,7 +985,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3">
@@ -993,31 +993,31 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <f>SUM(D10:D12)</f>
+        <f t="shared" ref="D9:J9" si="1">SUM(D10:D12)</f>
         <v>8</v>
       </c>
       <c r="E9" s="4">
-        <f>SUM(E10:E12)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F9" s="4">
-        <f>SUM(F10:F12)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G9" s="4">
-        <f>SUM(G10:G12)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H9" s="4">
-        <f>SUM(H10:H12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <f>SUM(I10:I12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="4">
-        <f>SUM(J10:J12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -1026,7 +1026,7 @@
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="25.5">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="6">
@@ -1064,7 +1064,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="25.5">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="6">
@@ -1102,7 +1102,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="38.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="6">
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="26.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="3">
@@ -1148,31 +1148,31 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:J13" si="0">SUM(D14:D17)</f>
+        <f t="shared" ref="D13:J13" si="2">SUM(D14:D17)</f>
         <v>12</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K13" s="5" t="s">
@@ -1181,7 +1181,7 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="25.5">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="6">
@@ -1219,7 +1219,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="6">
@@ -1257,7 +1257,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="25.5">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="6">
@@ -1295,7 +1295,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="25.5">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="6">
@@ -1333,7 +1333,7 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="3">
@@ -1345,27 +1345,27 @@
         <v>10</v>
       </c>
       <c r="E18" s="4">
-        <f>SUM(E19:E22)</f>
+        <f t="shared" ref="E18:J18" si="3">SUM(E19:E22)</f>
         <v>2</v>
       </c>
       <c r="F18" s="4">
-        <f>SUM(F19:F22)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G18" s="4">
-        <f>SUM(G19:G22)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H18" s="4">
-        <f>SUM(H19:H22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18" s="4">
-        <f>SUM(I19:I22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J18" s="4">
-        <f>SUM(J19:J22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -1374,7 +1374,7 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="25.5">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="6">
@@ -1412,7 +1412,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="25.5">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="6">
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="25.5">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="6">
@@ -1488,7 +1488,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="25.5">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="6">
@@ -1526,45 +1526,45 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="38.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="18">
         <v>8</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="22">
+      <c r="C23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="17">
         <v>3</v>
       </c>
-      <c r="E23" s="22">
-        <v>0</v>
-      </c>
-      <c r="F23" s="22">
-        <v>0</v>
-      </c>
-      <c r="G23" s="22">
-        <v>1</v>
-      </c>
-      <c r="H23" s="22">
-        <v>1</v>
-      </c>
-      <c r="I23" s="22">
-        <v>1</v>
-      </c>
-      <c r="J23" s="22">
+      <c r="E23" s="17">
+        <v>0</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0</v>
+      </c>
+      <c r="G23" s="17">
+        <v>1</v>
+      </c>
+      <c r="H23" s="17">
+        <v>1</v>
+      </c>
+      <c r="I23" s="17">
+        <v>1</v>
+      </c>
+      <c r="J23" s="17">
         <v>0</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="26.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="3">
@@ -1572,31 +1572,31 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4">
-        <f>SUM(D25:D27)</f>
+        <f t="shared" ref="D24:J24" si="4">SUM(D25:D27)</f>
         <v>5</v>
       </c>
       <c r="E24" s="4">
-        <f>SUM(E25:E27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F24" s="4">
-        <f>SUM(F25:F27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G24" s="4">
-        <f>SUM(G25:G27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H24" s="4">
-        <f>SUM(H25:H27)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I24" s="4">
-        <f>SUM(I25:I27)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J24" s="4">
-        <f>SUM(J25:J27)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -1605,7 +1605,7 @@
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" ht="25.5">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="6">
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="25.5">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="6">
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="25.5">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="6">
@@ -1719,7 +1719,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="12.75">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="9"/>
@@ -1777,84 +1777,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2277E5-F34C-48B9-8BB9-96917F3B1E32}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="20" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" style="20"/>
-    <col min="4" max="4" width="14.7109375" style="20" customWidth="1"/>
-    <col min="5" max="11" width="12.5703125" style="20"/>
-    <col min="12" max="12" width="13.85546875" style="20" customWidth="1"/>
-    <col min="13" max="16384" width="12.5703125" style="20"/>
+    <col min="1" max="1" width="17.42578125" style="15" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" style="15"/>
+    <col min="4" max="4" width="14.7109375" style="15" customWidth="1"/>
+    <col min="5" max="11" width="12.5703125" style="15"/>
+    <col min="12" max="12" width="13.85546875" style="15" customWidth="1"/>
+    <col min="13" max="16384" width="12.5703125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="14.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="25.5">
-      <c r="A3" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="19" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1862,913 +1862,913 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="21">
         <v>5</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="32">
+      <c r="C4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="22">
         <v>4</v>
       </c>
-      <c r="E4" s="32">
-        <f>SUM(E5:E6)</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="32">
-        <f>SUM(F5:F6)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="32">
-        <f>SUM(G5:G6)</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="32">
-        <f>SUM(H5:H6)</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="32">
-        <f>SUM(I5:I6)</f>
-        <v>1</v>
-      </c>
-      <c r="J4" s="32">
-        <f>SUM(J5:J6)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="33" t="s">
+      <c r="E4" s="22">
+        <f t="shared" ref="E4:J4" si="0">SUM(E5:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" ht="51">
+      <c r="A5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="24">
+        <v>5</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="38.25">
+      <c r="A6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="24">
+        <v>5</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
+      <c r="A7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="21">
         <v>13</v>
       </c>
-      <c r="L4" s="32"/>
-    </row>
-    <row r="5" spans="1:12" ht="51">
-      <c r="A5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="34">
+      <c r="C7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="22">
+        <f t="shared" ref="D7:J7" si="1">SUM(D8:D11)</f>
+        <v>10</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H7" s="22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="22">
+        <f>SUM(L5:L6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="38.25">
+      <c r="A8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="24">
+        <v>13</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="38.25">
+      <c r="A9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="24">
+        <v>13</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="38.25">
+      <c r="A10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="24">
+        <v>13</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="14">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="25.5">
+      <c r="A11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="24">
+        <v>13</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="39">
+      <c r="A12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="21">
         <v>5</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="19">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1</v>
-      </c>
-      <c r="F5" s="19">
-        <v>1</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="19">
-        <v>0</v>
-      </c>
-      <c r="I5" s="19">
-        <v>0</v>
-      </c>
-      <c r="J5" s="19">
-        <v>0</v>
-      </c>
-      <c r="K5" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="38.25">
-      <c r="A6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="34">
+      <c r="C12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="22">
+        <f t="shared" ref="D12:J12" si="2">SUM(D13:D16)</f>
+        <v>10</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="22">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="19">
-        <v>2</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="19">
-        <v>1</v>
-      </c>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
-      <c r="I6" s="19">
-        <v>1</v>
-      </c>
-      <c r="J6" s="19">
-        <v>0</v>
-      </c>
-      <c r="K6" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
-      <c r="A7" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="31">
-        <v>13</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="32">
-        <f t="shared" ref="D7:J7" si="0">SUM(D8:D11)</f>
-        <v>10</v>
-      </c>
-      <c r="E7" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G7" s="32">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H7" s="32">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I7" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J7" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="32">
-        <f>SUM(L5:L6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="38.25">
-      <c r="A8" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="34">
-        <v>13</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="19">
-        <v>4</v>
-      </c>
-      <c r="E8" s="19">
-        <v>2</v>
-      </c>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="38.25">
-      <c r="A9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="34">
-        <v>13</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="19">
-        <v>2</v>
-      </c>
-      <c r="E9" s="19">
-        <v>0</v>
-      </c>
-      <c r="F9" s="19">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>1</v>
-      </c>
-      <c r="H9" s="19">
-        <v>1</v>
-      </c>
-      <c r="I9" s="19">
-        <v>1</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="38.25">
-      <c r="A10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="34">
-        <v>13</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="19">
-        <v>2</v>
-      </c>
-      <c r="E10" s="19">
-        <v>0</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1</v>
-      </c>
-      <c r="H10" s="19">
-        <v>1</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="25.5">
-      <c r="A11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="34">
-        <v>13</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="19">
-        <v>2</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0</v>
-      </c>
-      <c r="F11" s="19">
-        <v>0</v>
-      </c>
-      <c r="G11" s="19">
-        <v>0</v>
-      </c>
-      <c r="H11" s="19">
-        <v>1</v>
-      </c>
-      <c r="I11" s="19">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="39">
-      <c r="A12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="31">
+      <c r="H12" s="22">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C12" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="32">
-        <f t="shared" ref="D12:J12" si="1">SUM(D13:D16)</f>
-        <v>10</v>
-      </c>
-      <c r="E12" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F12" s="32">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="G12" s="32">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H12" s="32">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I12" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J12" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="32">
+      <c r="I12" s="22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="22">
         <f>SUM(L8:L11)</f>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="38.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="24">
         <v>5</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="19">
+      <c r="C13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14">
         <v>3</v>
       </c>
-      <c r="E13" s="19">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19">
-        <v>1</v>
-      </c>
-      <c r="G13" s="19">
-        <v>1</v>
-      </c>
-      <c r="H13" s="19">
-        <v>0</v>
-      </c>
-      <c r="I13" s="19">
-        <v>0</v>
-      </c>
-      <c r="J13" s="19">
-        <v>0</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="19">
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+      <c r="G13" s="14">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.5">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="24">
         <v>5</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="E14" s="19">
-        <v>1</v>
-      </c>
-      <c r="F14" s="19">
+      <c r="C14" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
         <v>3</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="14">
         <v>3</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="14">
         <v>3</v>
       </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="19">
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="38.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="24">
         <v>5</v>
       </c>
-      <c r="C15" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="19">
-        <v>2</v>
-      </c>
-      <c r="E15" s="19">
-        <v>0</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
-        <v>1</v>
-      </c>
-      <c r="H15" s="19">
-        <v>1</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="19">
-        <v>0</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="19">
+      <c r="C15" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="14">
+        <v>2</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="51">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="24">
         <v>5</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="19">
+      <c r="C16" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="14">
         <v>3</v>
       </c>
-      <c r="E16" s="19">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
-        <v>0</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="19">
-        <v>1</v>
-      </c>
-      <c r="I16" s="19">
-        <v>2</v>
-      </c>
-      <c r="J16" s="19">
-        <v>0</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="19">
+      <c r="E16" s="14">
+        <v>0</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14">
+        <v>2</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="26.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="21">
         <v>13</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="32">
-        <f t="shared" ref="D17:J17" si="2">SUM(D18:D21)</f>
+      <c r="C17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="22">
+        <f t="shared" ref="D17:J17" si="3">SUM(D18:D21)</f>
         <v>14</v>
       </c>
-      <c r="E17" s="32">
-        <f t="shared" si="2"/>
+      <c r="E17" s="22">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F17" s="32">
-        <f t="shared" si="2"/>
+      <c r="F17" s="22">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G17" s="32">
-        <f t="shared" si="2"/>
+      <c r="G17" s="22">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="H17" s="32">
-        <f t="shared" si="2"/>
+      <c r="H17" s="22">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I17" s="32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J17" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="32">
+      <c r="I17" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="22">
         <f>SUM(L13:L16)</f>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="25.5">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="24">
         <v>13</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="19">
+      <c r="C18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14">
         <v>4</v>
       </c>
-      <c r="E18" s="19">
-        <v>2</v>
-      </c>
-      <c r="F18" s="19">
-        <v>1</v>
-      </c>
-      <c r="G18" s="19">
-        <v>1</v>
-      </c>
-      <c r="H18" s="19">
-        <v>0</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0</v>
-      </c>
-      <c r="J18" s="19">
-        <v>0</v>
-      </c>
-      <c r="K18" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L18" s="19">
+      <c r="E18" s="14">
+        <v>2</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.5">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="24">
         <v>13</v>
       </c>
-      <c r="C19" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="19">
+      <c r="C19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="14">
         <v>4</v>
       </c>
-      <c r="E19" s="19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="19">
-        <v>1</v>
-      </c>
-      <c r="I19" s="19">
-        <v>0</v>
-      </c>
-      <c r="J19" s="19">
-        <v>0</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="19">
+      <c r="E19" s="14">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="38.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="24">
         <v>13</v>
       </c>
-      <c r="C20" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="19">
+      <c r="C20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="14">
         <v>3</v>
       </c>
-      <c r="E20" s="19">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
-        <v>1</v>
-      </c>
-      <c r="G20" s="19">
-        <v>1</v>
-      </c>
-      <c r="H20" s="19">
-        <v>1</v>
-      </c>
-      <c r="I20" s="19">
-        <v>0</v>
-      </c>
-      <c r="J20" s="19">
-        <v>0</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L20" s="19">
+      <c r="E20" s="14">
+        <v>0</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="14">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="38.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="24">
         <v>13</v>
       </c>
-      <c r="C21" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="19">
+      <c r="C21" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="14">
         <v>3</v>
       </c>
-      <c r="E21" s="19">
-        <v>0</v>
-      </c>
-      <c r="F21" s="19">
-        <v>0</v>
-      </c>
-      <c r="G21" s="19">
-        <v>1</v>
-      </c>
-      <c r="H21" s="19">
-        <v>1</v>
-      </c>
-      <c r="I21" s="19">
-        <v>1</v>
-      </c>
-      <c r="J21" s="19">
-        <v>0</v>
-      </c>
-      <c r="K21" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="19">
+      <c r="E21" s="14">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14">
+        <v>1</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="26.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="21">
         <v>8</v>
       </c>
-      <c r="C22" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="32">
-        <f>SUM(D23:D25)</f>
+      <c r="C22" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="22">
+        <f t="shared" ref="D22:J22" si="4">SUM(D23:D25)</f>
         <v>8</v>
       </c>
-      <c r="E22" s="32">
-        <f>SUM(E23:E25)</f>
-        <v>2</v>
-      </c>
-      <c r="F22" s="32">
-        <f>SUM(F23:F25)</f>
-        <v>2</v>
-      </c>
-      <c r="G22" s="32">
-        <f>SUM(G23:G25)</f>
-        <v>2</v>
-      </c>
-      <c r="H22" s="32">
-        <f>SUM(H23:H25)</f>
-        <v>1</v>
-      </c>
-      <c r="I22" s="32">
-        <f>SUM(I23:I25)</f>
-        <v>1</v>
-      </c>
-      <c r="J22" s="32">
-        <f>SUM(J23:J25)</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="32">
+      <c r="E22" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F22" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="22">
         <f>SUM(L18:L21)</f>
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="38.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="24">
         <v>8</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="19">
-        <v>2</v>
-      </c>
-      <c r="E23" s="19">
-        <v>1</v>
-      </c>
-      <c r="F23" s="19">
-        <v>1</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="19">
-        <v>0</v>
-      </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L23" s="19">
+      <c r="C23" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="14">
+        <v>2</v>
+      </c>
+      <c r="E23" s="14">
+        <v>1</v>
+      </c>
+      <c r="F23" s="14">
+        <v>1</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0</v>
+      </c>
+      <c r="H23" s="14">
+        <v>0</v>
+      </c>
+      <c r="I23" s="14">
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
+        <v>0</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="51">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="24">
         <v>8</v>
       </c>
-      <c r="C24" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="19">
+      <c r="C24" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="14">
         <v>3</v>
       </c>
-      <c r="E24" s="19">
-        <v>1</v>
-      </c>
-      <c r="F24" s="19">
-        <v>0</v>
-      </c>
-      <c r="G24" s="19">
-        <v>1</v>
-      </c>
-      <c r="H24" s="19">
-        <v>1</v>
-      </c>
-      <c r="I24" s="19">
-        <v>0</v>
-      </c>
-      <c r="J24" s="19">
-        <v>0</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="19">
+      <c r="E24" s="14">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0</v>
+      </c>
+      <c r="G24" s="14">
+        <v>1</v>
+      </c>
+      <c r="H24" s="14">
+        <v>1</v>
+      </c>
+      <c r="I24" s="14">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="38.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="24">
         <v>8</v>
       </c>
-      <c r="C25" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="19">
+      <c r="C25" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="14">
         <v>3</v>
       </c>
-      <c r="E25" s="19">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19">
-        <v>1</v>
-      </c>
-      <c r="H25" s="19">
-        <v>0</v>
-      </c>
-      <c r="I25" s="19">
-        <v>1</v>
-      </c>
-      <c r="J25" s="19">
-        <v>0</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="19">
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+      <c r="G25" s="14">
+        <v>1</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
+        <v>1</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37">
-        <f>D4+D7+D12+D17+D22</f>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27">
+        <f t="shared" ref="D26:J26" si="5">D4+D7+D12+D17+D22</f>
         <v>46</v>
       </c>
-      <c r="E26" s="37">
-        <f>E4+E7+E12+E17+E22</f>
+      <c r="E26" s="27">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="F26" s="37">
-        <f>F4+F7+F12+F17+F22</f>
+      <c r="F26" s="27">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="G26" s="37">
-        <f>G4+G7+G12+G17+G22</f>
+      <c r="G26" s="27">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="H26" s="37">
-        <f>H4+H7+H12+H17+H22</f>
+      <c r="H26" s="27">
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="I26" s="37">
-        <f>I4+I7+I12+I17+I22</f>
+      <c r="I26" s="27">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="J26" s="37">
-        <f>J4+J7+J12+J17+J22</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="36"/>
-      <c r="L26" s="37">
+      <c r="J26" s="27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27">
         <f>SUM(L22,L17,L12,L7)</f>
         <v>14</v>
       </c>

</xml_diff>